<commit_message>
bugfixing and Pyromancy content
</commit_message>
<xml_diff>
--- a/Balance.xlsx
+++ b/Balance.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bartul\Documents\TowerOfElzair\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF15489E-583C-4B4E-B7ED-410FBD0E7BC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D156F3AC-FF2E-4AEC-B2FD-EC1B3EF7D3AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15975" yWindow="675" windowWidth="12435" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Abilities and values" sheetId="1" r:id="rId1"/>
+    <sheet name="Burn" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>General rules:</t>
   </si>
@@ -103,6 +104,45 @@
   </si>
   <si>
     <t>Adrenaline</t>
+  </si>
+  <si>
+    <t>Burn I</t>
+  </si>
+  <si>
+    <t>Burn II</t>
+  </si>
+  <si>
+    <t>Burn III</t>
+  </si>
+  <si>
+    <t>Burn IV</t>
+  </si>
+  <si>
+    <t>Burn V</t>
+  </si>
+  <si>
+    <t>Burn VI</t>
+  </si>
+  <si>
+    <t>Burn VII</t>
+  </si>
+  <si>
+    <t>Burn VIII</t>
+  </si>
+  <si>
+    <t>Burn IX</t>
+  </si>
+  <si>
+    <t>Burn X</t>
+  </si>
+  <si>
+    <t>Resistance</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Damage</t>
   </si>
 </sst>
 </file>
@@ -457,7 +497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -851,4 +891,767 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FD19AE0-4AFF-426F-B36A-CFF25440EAAE}">
+  <dimension ref="A1:M19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:M4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0.1</v>
+      </c>
+      <c r="E2">
+        <v>0.2</v>
+      </c>
+      <c r="F2">
+        <v>0.3</v>
+      </c>
+      <c r="G2">
+        <v>0.4</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>0.6</v>
+      </c>
+      <c r="J2">
+        <v>0.7</v>
+      </c>
+      <c r="K2">
+        <v>0.8</v>
+      </c>
+      <c r="L2">
+        <v>0.9</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>IF($A4*D$2-$B4&lt;=0,0,($A4*D$2-$B4)+IF(0.5*$A4*D$2-1.5*$B4&lt;=0,0,0.5*$A4*D$2-1.5*$B4)+IF(0.25*$A4*D$2-1.75*$B4&lt;=0,0,0.25*$A4*D$2-1.75*$B4+IF(0.125*$A4*D$2-1.875*$B4&lt;=0,0,0.125*$A4*D$2-1.875*$B4+IF(0.0625*$A4*D$2-1.9375*$B4&lt;=0,0,0.0625*$A4*D$2-1.9375*$B4))))</f>
+        <v>19.375</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:M10" si="0">IF($A4*E$2-$B4&lt;=0,0,($A4*E$2-$B4)+IF(0.5*$A4*E$2-1.5*$B4&lt;=0,0,0.5*$A4*E$2-1.5*$B4)+IF(0.25*$A4*E$2-1.75*$B4&lt;=0,0,0.25*$A4*E$2-1.75*$B4+IF(0.125*$A4*E$2-1.875*$B4&lt;=0,0,0.125*$A4*E$2-1.875*$B4+IF(0.0625*$A4*E$2-1.9375*$B4&lt;=0,0,0.0625*$A4*E$2-1.9375*$B4))))</f>
+        <v>38.75</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>58.125</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>77.5</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>96.875</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>116.25</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>135.625</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>155</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>174.375</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>193.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D10" si="1">IF($A5*D$2-$B5&lt;=0,0,($A5*D$2-$B5)+IF(0.5*$A5*D$2-1.5*$B5&lt;=0,0,0.5*$A5*D$2-1.5*$B5)+IF(0.25*$A5*D$2-1.75*$B5&lt;=0,0,0.25*$A5*D$2-1.75*$B5+IF(0.125*$A5*D$2-1.875*$B5&lt;=0,0,0.125*$A5*D$2-1.875*$B5+IF(0.0625*$A5*D$2-1.9375*$B5&lt;=0,0,0.0625*$A5*D$2-1.9375*$B5))))</f>
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>32.5</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>48.75</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>66.25</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>83.75</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>101.25</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>119.375</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>138.125</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>156.875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>100</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>97.5</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>115</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>132.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>100</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>37.5</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>52.5</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>67.5</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>82.5</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>97.5</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>100</v>
+      </c>
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>57.5</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>72.5</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>100</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f>IF($A13*D$2-$B13&lt;=0,0,($A13*D$2-$B13)+IF(0.5*$A13*D$2-1.5*$B13&lt;=0,0,0.5*$A13*D$2-1.5*$B13)+IF(0.25*$A13*D$2-1.75*$B13&lt;=0,0,0.25*$A13*D$2-1.75*$B13+IF(0.125*$A13*D$2-1.875*$B13&lt;=0,0,0.125*$A13*D$2-1.875*$B13+IF(0.0625*$A13*D$2-1.9375*$B13&lt;=0,0,0.0625*$A13*D$2-1.9375*$B13))))</f>
+        <v>9.6875</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:M19" si="2">IF($A13*E$2-$B13&lt;=0,0,($A13*E$2-$B13)+IF(0.5*$A13*E$2-1.5*$B13&lt;=0,0,0.5*$A13*E$2-1.5*$B13)+IF(0.25*$A13*E$2-1.75*$B13&lt;=0,0,0.25*$A13*E$2-1.75*$B13+IF(0.125*$A13*E$2-1.875*$B13&lt;=0,0,0.125*$A13*E$2-1.875*$B13+IF(0.0625*$A13*E$2-1.9375*$B13&lt;=0,0,0.0625*$A13*E$2-1.9375*$B13))))</f>
+        <v>19.375</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>29.0625</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>38.75</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>48.4375</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>58.125</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>67.8125</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>77.5</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>87.1875</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>96.875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:D19" si="3">IF($A14*D$2-$B14&lt;=0,0,($A14*D$2-$B14)+IF(0.5*$A14*D$2-1.5*$B14&lt;=0,0,0.5*$A14*D$2-1.5*$B14)+IF(0.25*$A14*D$2-1.75*$B14&lt;=0,0,0.25*$A14*D$2-1.75*$B14+IF(0.125*$A14*D$2-1.875*$B14&lt;=0,0,0.125*$A14*D$2-1.875*$B14+IF(0.0625*$A14*D$2-1.9375*$B14&lt;=0,0,0.0625*$A14*D$2-1.9375*$B14))))</f>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>17.5</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>32.5</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>48.75</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>57.5</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>66.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>27.5</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>42.5</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>50</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>50</v>
+      </c>
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>50</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>